<commit_message>
Fix error get result from test term classification and write into logs.xlsx
</commit_message>
<xml_diff>
--- a/20160311 - 004/running_logs/logs.xlsx
+++ b/20160311 - 004/running_logs/logs.xlsx
@@ -407,13 +407,10 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>